<commit_message>
Added missing sub industries
</commit_message>
<xml_diff>
--- a/gics.xlsx
+++ b/gics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/LaCie/Dev/global-industry-classification-standard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6836DD12-DDC4-F448-8825-B0102A7D2FE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBBFBE7-0471-5245-974B-450087D5DF13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1460" windowWidth="43320" windowHeight="22180" activeTab="3" xr2:uid="{1D78C696-9476-5D43-A873-93FD977A96B5}"/>
+    <workbookView xWindow="18960" yWindow="2980" windowWidth="31080" windowHeight="21400" activeTab="3" xr2:uid="{1D78C696-9476-5D43-A873-93FD977A96B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sector" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="233">
   <si>
     <t>Sector</t>
   </si>
@@ -721,6 +721,12 @@
   </si>
   <si>
     <t xml:space="preserve">Mortgage Real Estate Investment </t>
+  </si>
+  <si>
+    <t>Financial Exchanges &amp; Data</t>
+  </si>
+  <si>
+    <t>Mortgage REITs</t>
   </si>
 </sst>
 </file>
@@ -2274,10 +2280,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B12EA4-2E76-DB48-8110-AD8ABCB683F1}">
-  <dimension ref="A1:C157"/>
+  <dimension ref="A1:C159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D164" sqref="D164"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3509,24 +3515,24 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>403010</v>
+        <v>402030</v>
       </c>
       <c r="B112">
-        <v>40301010</v>
+        <v>40203040</v>
       </c>
       <c r="C112" t="s">
-        <v>158</v>
+        <v>231</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>403010</v>
+        <v>402040</v>
       </c>
       <c r="B113">
-        <v>40301020</v>
+        <v>40204010</v>
       </c>
       <c r="C113" t="s">
-        <v>159</v>
+        <v>232</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -3534,10 +3540,10 @@
         <v>403010</v>
       </c>
       <c r="B114">
-        <v>40301030</v>
+        <v>40301010</v>
       </c>
       <c r="C114" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -3545,10 +3551,10 @@
         <v>403010</v>
       </c>
       <c r="B115">
-        <v>40301040</v>
+        <v>40301020</v>
       </c>
       <c r="C115" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -3556,32 +3562,32 @@
         <v>403010</v>
       </c>
       <c r="B116">
-        <v>40301050</v>
+        <v>40301030</v>
       </c>
       <c r="C116" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117">
-        <v>451020</v>
+        <v>403010</v>
       </c>
       <c r="B117">
-        <v>45102010</v>
+        <v>40301040</v>
       </c>
       <c r="C117" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118">
-        <v>451020</v>
+        <v>403010</v>
       </c>
       <c r="B118">
-        <v>45102020</v>
+        <v>40301050</v>
       </c>
       <c r="C118" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -3589,76 +3595,76 @@
         <v>451020</v>
       </c>
       <c r="B119">
-        <v>45102030</v>
+        <v>45102010</v>
       </c>
       <c r="C119" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120">
-        <v>451030</v>
+        <v>451020</v>
       </c>
       <c r="B120">
-        <v>45103010</v>
+        <v>45102020</v>
       </c>
       <c r="C120" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121">
-        <v>451030</v>
+        <v>451020</v>
       </c>
       <c r="B121">
-        <v>45103020</v>
+        <v>45102030</v>
       </c>
       <c r="C121" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122">
-        <v>452010</v>
+        <v>451030</v>
       </c>
       <c r="B122">
-        <v>45201020</v>
+        <v>45103010</v>
       </c>
       <c r="C122" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123">
-        <v>452020</v>
+        <v>451030</v>
       </c>
       <c r="B123">
-        <v>45202030</v>
+        <v>45103020</v>
       </c>
       <c r="C123" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124">
-        <v>452030</v>
+        <v>452010</v>
       </c>
       <c r="B124">
-        <v>45203010</v>
+        <v>45201020</v>
       </c>
       <c r="C124" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125">
-        <v>452030</v>
+        <v>452020</v>
       </c>
       <c r="B125">
-        <v>45203015</v>
+        <v>45202030</v>
       </c>
       <c r="C125" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
@@ -3666,10 +3672,10 @@
         <v>452030</v>
       </c>
       <c r="B126">
-        <v>45203020</v>
+        <v>45203010</v>
       </c>
       <c r="C126" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
@@ -3677,87 +3683,87 @@
         <v>452030</v>
       </c>
       <c r="B127">
-        <v>45203030</v>
+        <v>45203015</v>
       </c>
       <c r="C127" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128">
-        <v>453010</v>
+        <v>452030</v>
       </c>
       <c r="B128">
-        <v>45301010</v>
+        <v>45203020</v>
       </c>
       <c r="C128" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129">
-        <v>453010</v>
+        <v>452030</v>
       </c>
       <c r="B129">
-        <v>45301020</v>
+        <v>45203030</v>
       </c>
       <c r="C129" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130">
-        <v>501010</v>
+        <v>453010</v>
       </c>
       <c r="B130">
-        <v>50101010</v>
+        <v>45301010</v>
       </c>
       <c r="C130" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131">
-        <v>501010</v>
+        <v>453010</v>
       </c>
       <c r="B131">
-        <v>50101020</v>
+        <v>45301020</v>
       </c>
       <c r="C131" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132">
-        <v>501020</v>
+        <v>501010</v>
       </c>
       <c r="B132">
-        <v>50102010</v>
+        <v>50101010</v>
       </c>
       <c r="C132" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133">
-        <v>502010</v>
+        <v>501010</v>
       </c>
       <c r="B133">
-        <v>50201010</v>
+        <v>50101020</v>
       </c>
       <c r="C133" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134">
-        <v>502010</v>
+        <v>501020</v>
       </c>
       <c r="B134">
-        <v>50201020</v>
+        <v>50102010</v>
       </c>
       <c r="C134" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
@@ -3765,10 +3771,10 @@
         <v>502010</v>
       </c>
       <c r="B135">
-        <v>50201030</v>
+        <v>50201010</v>
       </c>
       <c r="C135" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
@@ -3776,131 +3782,131 @@
         <v>502010</v>
       </c>
       <c r="B136">
-        <v>50201040</v>
+        <v>50201020</v>
       </c>
       <c r="C136" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137">
-        <v>502020</v>
+        <v>502010</v>
       </c>
       <c r="B137">
-        <v>50202010</v>
+        <v>50201030</v>
       </c>
       <c r="C137" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138">
-        <v>502020</v>
+        <v>502010</v>
       </c>
       <c r="B138">
-        <v>50202020</v>
+        <v>50201040</v>
       </c>
       <c r="C138" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139">
-        <v>502030</v>
+        <v>502020</v>
       </c>
       <c r="B139">
-        <v>50203010</v>
+        <v>50202010</v>
       </c>
       <c r="C139" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140">
-        <v>551010</v>
+        <v>502020</v>
       </c>
       <c r="B140">
-        <v>55101010</v>
+        <v>50202020</v>
       </c>
       <c r="C140" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141">
-        <v>551020</v>
+        <v>502030</v>
       </c>
       <c r="B141">
-        <v>55102010</v>
+        <v>50203010</v>
       </c>
       <c r="C141" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142">
-        <v>551030</v>
+        <v>551010</v>
       </c>
       <c r="B142">
-        <v>55103010</v>
+        <v>55101010</v>
       </c>
       <c r="C142" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143">
-        <v>551040</v>
+        <v>551020</v>
       </c>
       <c r="B143">
-        <v>55104010</v>
+        <v>55102010</v>
       </c>
       <c r="C143" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144">
-        <v>551050</v>
+        <v>551030</v>
       </c>
       <c r="B144">
-        <v>55105010</v>
+        <v>55103010</v>
       </c>
       <c r="C144" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145">
-        <v>551050</v>
+        <v>551040</v>
       </c>
       <c r="B145">
-        <v>55105020</v>
+        <v>55104010</v>
       </c>
       <c r="C145" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146">
-        <v>601010</v>
+        <v>551050</v>
       </c>
       <c r="B146">
-        <v>60101010</v>
+        <v>55105010</v>
       </c>
       <c r="C146" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147">
-        <v>601010</v>
+        <v>551050</v>
       </c>
       <c r="B147">
-        <v>60101020</v>
+        <v>55105020</v>
       </c>
       <c r="C147" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
@@ -3908,10 +3914,10 @@
         <v>601010</v>
       </c>
       <c r="B148">
-        <v>60101030</v>
+        <v>60101010</v>
       </c>
       <c r="C148" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
@@ -3919,10 +3925,10 @@
         <v>601010</v>
       </c>
       <c r="B149">
-        <v>60101040</v>
+        <v>60101020</v>
       </c>
       <c r="C149" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
@@ -3930,10 +3936,10 @@
         <v>601010</v>
       </c>
       <c r="B150">
-        <v>60101050</v>
+        <v>60101030</v>
       </c>
       <c r="C150" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
@@ -3941,10 +3947,10 @@
         <v>601010</v>
       </c>
       <c r="B151">
-        <v>60101060</v>
+        <v>60101040</v>
       </c>
       <c r="C151" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
@@ -3952,10 +3958,10 @@
         <v>601010</v>
       </c>
       <c r="B152">
-        <v>60101070</v>
+        <v>60101050</v>
       </c>
       <c r="C152" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
@@ -3963,32 +3969,32 @@
         <v>601010</v>
       </c>
       <c r="B153">
-        <v>60101080</v>
+        <v>60101060</v>
       </c>
       <c r="C153" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154">
-        <v>601020</v>
+        <v>601010</v>
       </c>
       <c r="B154">
-        <v>60102010</v>
+        <v>60101070</v>
       </c>
       <c r="C154" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155">
-        <v>601020</v>
+        <v>601010</v>
       </c>
       <c r="B155">
-        <v>60102020</v>
+        <v>60101080</v>
       </c>
       <c r="C155" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
@@ -3996,10 +4002,10 @@
         <v>601020</v>
       </c>
       <c r="B156">
-        <v>60102030</v>
+        <v>60102010</v>
       </c>
       <c r="C156" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
@@ -4007,9 +4013,31 @@
         <v>601020</v>
       </c>
       <c r="B157">
+        <v>60102020</v>
+      </c>
+      <c r="C157" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>601020</v>
+      </c>
+      <c r="B158">
+        <v>60102030</v>
+      </c>
+      <c r="C158" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>601020</v>
+      </c>
+      <c r="B159">
         <v>60102040</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C159" t="s">
         <v>221</v>
       </c>
     </row>

</xml_diff>